<commit_message>
Updated data_reference.txt and exploratory-analysis.xlsx
</commit_message>
<xml_diff>
--- a/workbench/exploratory-analysis.xlsx
+++ b/workbench/exploratory-analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Desktop\MTech EBAC Sem 1\Practice Module\F5-APM\workbench\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{679D48D8-6F14-4430-923C-6B162293A0F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A25CD456-C5A8-438D-9DC5-633DFE55D1B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SG Overall GDP Growth" sheetId="5" r:id="rId1"/>
@@ -31,8 +31,8 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId10"/>
-    <pivotCache cacheId="0" r:id="rId11"/>
+    <pivotCache cacheId="0" r:id="rId10"/>
+    <pivotCache cacheId="1" r:id="rId11"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="38">
   <si>
     <t>Year</t>
   </si>
@@ -175,6 +175,9 @@
   <si>
     <t xml:space="preserve">         Accommodation &amp; Food Services </t>
   </si>
+  <si>
+    <t>2019</t>
+  </si>
 </sst>
 </file>
 
@@ -234,7 +237,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -266,12 +269,97 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="28">
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
     <dxf>
       <alignment vertical="center"/>
     </dxf>
@@ -340,7 +428,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-SG" baseline="0"/>
-              <a:t> Overall GDP (2013 - 2020)</a:t>
+              <a:t> Overall GDP Growth Rate (%)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -582,9 +670,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'SG Overall GDP Growth'!$A$4:$A$9</c:f>
+              <c:f>'SG Overall GDP Growth'!$A$4:$A$10</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>2013</c:v>
                 </c:pt>
@@ -602,16 +690,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2019</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'SG Overall GDP Growth'!$B$4:$B$9</c:f>
+              <c:f>'SG Overall GDP Growth'!$B$4:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>4.8000000000000007</c:v>
                 </c:pt>
@@ -629,6 +720,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>3.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -863,7 +957,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-SG"/>
-              <a:t>SG GDP Growth by Sector (2013 - 2018)</a:t>
+              <a:t>SG GDP Growth by Sector (%)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2535,7 +2629,7 @@
           <c:yMode val="edge"/>
           <c:x val="4.1559764861927938E-2"/>
           <c:y val="0.13668689602820078"/>
-          <c:w val="0.52234986392902005"/>
+          <c:w val="0.65521148013014163"/>
           <c:h val="0.82277506524680033"/>
         </c:manualLayout>
       </c:layout>
@@ -2570,9 +2664,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'SG GDP Growth by Sector'!$A$5:$A$10</c:f>
+              <c:f>'SG GDP Growth by Sector'!$A$5:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>2013</c:v>
                 </c:pt>
@@ -2590,16 +2684,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2019</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'SG GDP Growth by Sector'!$B$5:$B$10</c:f>
+              <c:f>'SG GDP Growth by Sector'!$B$5:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0.1</c:v>
                 </c:pt>
@@ -2617,6 +2714,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2656,9 +2756,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'SG GDP Growth by Sector'!$A$5:$A$10</c:f>
+              <c:f>'SG GDP Growth by Sector'!$A$5:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>2013</c:v>
                 </c:pt>
@@ -2676,16 +2776,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2019</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'SG GDP Growth by Sector'!$C$5:$C$10</c:f>
+              <c:f>'SG GDP Growth by Sector'!$C$5:$C$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0.1</c:v>
                 </c:pt>
@@ -2703,6 +2806,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2742,9 +2848,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'SG GDP Growth by Sector'!$A$5:$A$10</c:f>
+              <c:f>'SG GDP Growth by Sector'!$A$5:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>2013</c:v>
                 </c:pt>
@@ -2762,16 +2868,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2019</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'SG GDP Growth by Sector'!$D$5:$D$10</c:f>
+              <c:f>'SG GDP Growth by Sector'!$D$5:$D$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1.8</c:v>
                 </c:pt>
@@ -2789,6 +2898,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2828,9 +2940,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'SG GDP Growth by Sector'!$A$5:$A$10</c:f>
+              <c:f>'SG GDP Growth by Sector'!$A$5:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>2013</c:v>
                 </c:pt>
@@ -2848,16 +2960,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2019</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'SG GDP Growth by Sector'!$E$5:$E$10</c:f>
+              <c:f>'SG GDP Growth by Sector'!$E$5:$E$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0.3</c:v>
                 </c:pt>
@@ -2875,6 +2990,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2914,9 +3032,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'SG GDP Growth by Sector'!$A$5:$A$10</c:f>
+              <c:f>'SG GDP Growth by Sector'!$A$5:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>2013</c:v>
                 </c:pt>
@@ -2934,16 +3052,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2019</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'SG GDP Growth by Sector'!$F$5:$F$10</c:f>
+              <c:f>'SG GDP Growth by Sector'!$F$5:$F$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0.3</c:v>
                 </c:pt>
@@ -2961,6 +3082,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3000,9 +3124,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'SG GDP Growth by Sector'!$A$5:$A$10</c:f>
+              <c:f>'SG GDP Growth by Sector'!$A$5:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>2013</c:v>
                 </c:pt>
@@ -3020,16 +3144,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2019</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'SG GDP Growth by Sector'!$G$5:$G$10</c:f>
+              <c:f>'SG GDP Growth by Sector'!$G$5:$G$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -3046,6 +3173,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -3088,9 +3218,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'SG GDP Growth by Sector'!$A$5:$A$10</c:f>
+              <c:f>'SG GDP Growth by Sector'!$A$5:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>2013</c:v>
                 </c:pt>
@@ -3108,16 +3238,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2019</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'SG GDP Growth by Sector'!$H$5:$H$10</c:f>
+              <c:f>'SG GDP Growth by Sector'!$H$5:$H$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0.2</c:v>
                 </c:pt>
@@ -3135,6 +3268,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3176,9 +3312,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'SG GDP Growth by Sector'!$A$5:$A$10</c:f>
+              <c:f>'SG GDP Growth by Sector'!$A$5:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>2013</c:v>
                 </c:pt>
@@ -3196,16 +3332,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2019</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'SG GDP Growth by Sector'!$I$5:$I$10</c:f>
+              <c:f>'SG GDP Growth by Sector'!$I$5:$I$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0.7</c:v>
                 </c:pt>
@@ -3223,6 +3362,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3264,9 +3406,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'SG GDP Growth by Sector'!$A$5:$A$10</c:f>
+              <c:f>'SG GDP Growth by Sector'!$A$5:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>2013</c:v>
                 </c:pt>
@@ -3284,16 +3426,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2019</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'SG GDP Growth by Sector'!$J$5:$J$10</c:f>
+              <c:f>'SG GDP Growth by Sector'!$J$5:$J$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0.2</c:v>
                 </c:pt>
@@ -3310,6 +3455,9 @@
                   <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -3352,9 +3500,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'SG GDP Growth by Sector'!$A$5:$A$10</c:f>
+              <c:f>'SG GDP Growth by Sector'!$A$5:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>2013</c:v>
                 </c:pt>
@@ -3372,16 +3520,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2019</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'SG GDP Growth by Sector'!$K$5:$K$10</c:f>
+              <c:f>'SG GDP Growth by Sector'!$K$5:$K$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -3398,6 +3549,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -3440,9 +3594,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'SG GDP Growth by Sector'!$A$5:$A$10</c:f>
+              <c:f>'SG GDP Growth by Sector'!$A$5:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>2013</c:v>
                 </c:pt>
@@ -3460,16 +3614,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2019</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'SG GDP Growth by Sector'!$L$5:$L$10</c:f>
+              <c:f>'SG GDP Growth by Sector'!$L$5:$L$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1.1000000000000001</c:v>
                 </c:pt>
@@ -3487,6 +3644,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3631,9 +3791,9 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.58305142415545586"/>
+          <c:x val="0.72151410533326821"/>
           <c:y val="8.1505148670290253E-2"/>
-          <c:w val="0.40732468074664457"/>
+          <c:w val="0.26886189234547392"/>
           <c:h val="0.89918594595798296"/>
         </c:manualLayout>
       </c:layout>
@@ -10851,8 +11011,8 @@
       <xdr:rowOff>78104</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>87630</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1125071</xdr:colOff>
       <xdr:row>35</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -11057,8 +11217,8 @@
       <sheetName val="GDP Total"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
       <sheetData sheetId="2">
         <row r="1">
           <cell r="B1" t="str">
@@ -11114,7 +11274,7 @@
       <sheetName val="processed"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
+      <sheetData sheetId="0" refreshError="1"/>
       <sheetData sheetId="1">
         <row r="1">
           <cell r="C1" t="str">
@@ -11176,11 +11336,11 @@
       <sheetName val="grad-employment rate by cluster"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
       <sheetData sheetId="5">
         <row r="1">
           <cell r="D1" t="str">
@@ -11223,8 +11383,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -19836,8 +19996,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{110B1438-09B8-49FD-8355-CED3694DB390}" name="PivotTable2" cacheId="0" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
-  <location ref="A3:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{110B1438-09B8-49FD-8355-CED3694DB390}" name="PivotTable2" cacheId="1" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+  <location ref="A3:B10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -19867,13 +20027,13 @@
     <pivotField dataField="1" showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
     <pivotField showAll="0"/>
   </pivotFields>
   <rowFields count="1">
     <field x="-2"/>
   </rowFields>
-  <rowItems count="6">
+  <rowItems count="7">
     <i>
       <x/>
     </i>
@@ -19892,17 +20052,21 @@
     <i i="5">
       <x v="5"/>
     </i>
+    <i i="6">
+      <x v="6"/>
+    </i>
   </rowItems>
   <colItems count="1">
     <i/>
   </colItems>
-  <dataFields count="6">
+  <dataFields count="7">
     <dataField name="2013" fld="3" baseField="0" baseItem="0"/>
     <dataField name="2014" fld="4" baseField="0" baseItem="0"/>
     <dataField name="2015" fld="5" baseField="0" baseItem="0"/>
     <dataField name="2016" fld="6" baseField="0" baseItem="0"/>
     <dataField name="2017" fld="7" baseField="0" baseItem="0"/>
     <dataField name="2018" fld="8" baseField="0" baseItem="0"/>
+    <dataField name="2019" fld="9" baseField="0" baseItem="0"/>
   </dataFields>
   <chartFormats count="2">
     <chartFormat chart="1" format="0" series="1">
@@ -19937,8 +20101,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D8D8D958-CA9C-4544-8C86-1853F15E3A50}" name="PivotTable3" cacheId="0" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7">
-  <location ref="A3:M10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D8D8D958-CA9C-4544-8C86-1853F15E3A50}" name="PivotTable3" cacheId="1" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7">
+  <location ref="A3:M11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField showAll="0">
       <items count="3">
@@ -19981,13 +20145,13 @@
     <pivotField dataField="1" showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
     <pivotField showAll="0"/>
   </pivotFields>
   <rowFields count="1">
     <field x="-2"/>
   </rowFields>
-  <rowItems count="6">
+  <rowItems count="7">
     <i>
       <x/>
     </i>
@@ -20005,6 +20169,9 @@
     </i>
     <i i="5">
       <x v="5"/>
+    </i>
+    <i i="6">
+      <x v="6"/>
     </i>
   </rowItems>
   <colFields count="1">
@@ -20048,14 +20215,233 @@
       <x/>
     </i>
   </colItems>
-  <dataFields count="6">
+  <dataFields count="7">
     <dataField name="2013" fld="3" baseField="0" baseItem="0"/>
     <dataField name="2014" fld="4" baseField="0" baseItem="0"/>
     <dataField name="2015" fld="5" baseField="0" baseItem="0"/>
     <dataField name="2016" fld="6" baseField="0" baseItem="0"/>
     <dataField name="2017" fld="7" baseField="0" baseItem="0"/>
     <dataField name="2018" fld="8" baseField="0" baseItem="0"/>
+    <dataField name="2019" fld="9" baseField="0" baseItem="0"/>
   </dataFields>
+  <formats count="24">
+    <format dxfId="23">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="22">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="21">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="20">
+      <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="19">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="18">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="17">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="16">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="15">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="14">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="13">
+      <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="12">
+      <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="11">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="10">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="9">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="8">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="7">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="6">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="5">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="8"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="4">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="8"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="3">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="9"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="2">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="9"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="1">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="10"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="0">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="10"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
   <chartFormats count="22">
     <chartFormat chart="1" format="14" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
@@ -20317,7 +20703,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{459F7DD8-E4DD-4E23-95A5-1514C71FF386}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{459F7DD8-E4DD-4E23-95A5-1514C71FF386}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1" fieldListSortAscending="1">
   <location ref="A2:B10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField axis="axisRow" showAll="0">
@@ -20377,7 +20763,7 @@
     <dataField name="Average of employment_rate_overall" fld="4" subtotal="average" baseField="0" baseItem="0" numFmtId="2"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="3">
+    <format dxfId="27">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -20405,7 +20791,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AFC0F0E9-3665-43CA-A3EC-E98920C57017}" name="PivotTable4" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AFC0F0E9-3665-43CA-A3EC-E98920C57017}" name="PivotTable4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4" fieldListSortAscending="1">
   <location ref="A1:J10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField axis="axisRow" showAll="0">
@@ -20506,13 +20892,13 @@
     <dataField name="Average of employment_rate_overall" fld="4" subtotal="average" baseField="0" baseItem="0" numFmtId="2"/>
   </dataFields>
   <formats count="3">
-    <format dxfId="2">
+    <format dxfId="26">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="1">
+    <format dxfId="25">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="0">
+    <format dxfId="24">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
   </formats>
@@ -20889,10 +21275,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5D2A7F3-3707-4777-AA68-30A675F812EA}">
-  <dimension ref="A3:B9"/>
+  <dimension ref="A3:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -20903,7 +21289,7 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
+      <c r="A3" s="12" t="s">
         <v>19</v>
       </c>
     </row>
@@ -20911,7 +21297,7 @@
       <c r="A4" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="17">
         <v>4.8000000000000007</v>
       </c>
     </row>
@@ -20919,7 +21305,7 @@
       <c r="A5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="17">
         <v>3.5999999999999996</v>
       </c>
     </row>
@@ -20927,7 +21313,7 @@
       <c r="A6" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="17">
         <v>2.1999999999999997</v>
       </c>
     </row>
@@ -20935,7 +21321,7 @@
       <c r="A7" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="17">
         <v>2.2000000000000002</v>
       </c>
     </row>
@@ -20943,7 +21329,7 @@
       <c r="A8" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="17">
         <v>3.9</v>
       </c>
     </row>
@@ -20951,8 +21337,16 @@
       <c r="A9" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="17">
         <v>3.3000000000000007</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="17">
+        <v>1.2</v>
       </c>
     </row>
   </sheetData>
@@ -20963,25 +21357,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20BA367D-A17B-4F22-A127-963AB76BCD3C}">
-  <dimension ref="A3:M10"/>
+  <dimension ref="A3:M11"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="11.578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.68359375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.3671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.3671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="25.3671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="64.3125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.62890625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.20703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.62890625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.9453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1015625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7890625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.1015625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.89453125" customWidth="1"/>
+    <col min="8" max="8" width="16.3125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32.3671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.68359375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.1015625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.20703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -20990,41 +21385,41 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:13" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" s="16" t="s">
         <v>26</v>
       </c>
       <c r="M4" t="s">
@@ -21035,40 +21430,40 @@
       <c r="A5" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="18">
         <v>0.1</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="17">
         <v>0.1</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="17">
         <v>1.8</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="17">
         <v>0.3</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="19">
         <v>0.3</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="17">
         <v>0</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="17">
         <v>0.2</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="17">
         <v>0.7</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="17">
         <v>0.2</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="17">
         <v>0</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="17">
         <v>1.1000000000000001</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="17">
         <v>4.8000000000000007</v>
       </c>
     </row>
@@ -21076,40 +21471,40 @@
       <c r="A6" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="18">
         <v>0</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="17">
         <v>0.4</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="17">
         <v>1</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="17">
         <v>0.3</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="19">
         <v>0.5</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="17">
         <v>0</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="17">
         <v>0.3</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="17">
         <v>0.30000000000000004</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="17">
         <v>0.1</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="17">
         <v>0</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="17">
         <v>0.7</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="17">
         <v>3.5999999999999996</v>
       </c>
     </row>
@@ -21117,40 +21512,40 @@
       <c r="A7" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="18">
         <v>0</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="17">
         <v>0.3</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="17">
         <v>0.5</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="17">
         <v>0</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="19">
         <v>-0.9</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="17">
         <v>0</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="17">
         <v>0.3</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="17">
         <v>1.2</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="17">
         <v>0.2</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="17">
         <v>0</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="17">
         <v>0.6</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="17">
         <v>2.1999999999999997</v>
       </c>
     </row>
@@ -21158,40 +21553,40 @@
       <c r="A8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="18">
         <v>0</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="17">
         <v>-0.1</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="17">
         <v>0.1</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="17">
         <v>0.2</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="19">
         <v>0.7</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="17">
         <v>0</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="17">
         <v>0.4</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="17">
         <v>0.7</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="17">
         <v>0.1</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="17">
         <v>0</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="17">
         <v>0.1</v>
       </c>
-      <c r="M8">
+      <c r="M8" s="17">
         <v>2.1999999999999997</v>
       </c>
     </row>
@@ -21199,40 +21594,40 @@
       <c r="A9" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="18">
         <v>0</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="17">
         <v>-0.2</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="17">
         <v>0.9</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="17">
         <v>0.3</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="19">
         <v>1.8</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="17">
         <v>0</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="17">
         <v>0.3</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="17">
         <v>0.2</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="17">
         <v>0.3</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="17">
         <v>0</v>
       </c>
-      <c r="L9">
+      <c r="L9" s="17">
         <v>0.3</v>
       </c>
-      <c r="M9">
+      <c r="M9" s="17">
         <v>3.8999999999999995</v>
       </c>
     </row>
@@ -21240,41 +21635,82 @@
       <c r="A10" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="18">
         <v>0.1</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="17">
         <v>0</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="17">
         <v>0.7</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="17">
         <v>0.2</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="19">
         <v>1.3</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="17">
         <v>0</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="17">
         <v>0.2</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="17">
         <v>0.4</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="17">
         <v>0</v>
       </c>
-      <c r="K10">
+      <c r="K10" s="17">
         <v>0</v>
       </c>
-      <c r="L10">
+      <c r="L10" s="17">
         <v>0.4</v>
       </c>
-      <c r="M10">
+      <c r="M10" s="17">
         <v>3.3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="18">
+        <v>0</v>
+      </c>
+      <c r="C11" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="D11" s="17">
+        <v>1</v>
+      </c>
+      <c r="E11" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="F11" s="19">
+        <v>-0.3</v>
+      </c>
+      <c r="G11" s="17">
+        <v>0</v>
+      </c>
+      <c r="H11" s="17">
+        <v>0.4</v>
+      </c>
+      <c r="I11" s="17">
+        <v>-0.4</v>
+      </c>
+      <c r="J11" s="17">
+        <v>0</v>
+      </c>
+      <c r="K11" s="17">
+        <v>0</v>
+      </c>
+      <c r="L11" s="17">
+        <v>-0.1</v>
+      </c>
+      <c r="M11" s="17">
+        <v>1.2000000000000002</v>
       </c>
     </row>
   </sheetData>
@@ -21288,7 +21724,7 @@
   <dimension ref="A2:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -21381,8 +21817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F508B9FF-68B0-4E9B-AB7E-9C705EC58C14}">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -21704,7 +22140,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -21875,8 +22311,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{134DC496-8FC5-4225-BA33-085BD38A64CD}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -21884,7 +22320,7 @@
     <col min="1" max="1" width="16.15625" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="15.5234375" customWidth="1"/>
-    <col min="4" max="4" width="10.41796875" customWidth="1"/>
+    <col min="4" max="4" width="12.41796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="43.2" x14ac:dyDescent="0.55000000000000004">

</xml_diff>